<commit_message>
--- TERREMOTO NO BRASIL ---
</commit_message>
<xml_diff>
--- a/sismos_Brazil.xlsx
+++ b/sismos_Brazil.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="sismos_Brazil" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="ORDEM DE DATA - GRÁFICOS" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="ORDEM DE MAG" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="219">
   <si>
     <t xml:space="preserve">SISMOS NO BRASIL (&gt;5)</t>
   </si>
@@ -656,6 +657,54 @@
   </si>
   <si>
     <t xml:space="preserve">04:40:08.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAG.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOCAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAÍS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HORA</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mapa: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://earthquake.usgs.gov/earthquakes/eventpage/*********/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">executive#map</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -666,7 +715,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -699,6 +748,20 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -743,7 +806,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -756,7 +819,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -766,6 +829,18 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -874,7 +949,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>sismos_Brazil!$A$2:$A$67</c:f>
+              <c:f>'ORDEM DE DATA - GRÁFICOS'!$A$2:$A$67</c:f>
               <c:strCache>
                 <c:ptCount val="66"/>
                 <c:pt idx="0">
@@ -1080,7 +1155,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>sismos_Brazil!$B$2:$B$67</c:f>
+              <c:f>'ORDEM DE DATA - GRÁFICOS'!$B$2:$B$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="66"/>
@@ -1288,11 +1363,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="83152997"/>
-        <c:axId val="16404224"/>
+        <c:axId val="70834426"/>
+        <c:axId val="34742880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="83152997"/>
+        <c:axId val="70834426"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1320,14 +1395,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16404224"/>
+        <c:crossAx val="34742880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="16404224"/>
+        <c:axId val="34742880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1364,7 +1439,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83152997"/>
+        <c:crossAx val="70834426"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1428,7 +1503,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>sismos_Brazil!$A$2:$A$67</c:f>
+              <c:f>'ORDEM DE DATA - GRÁFICOS'!$A$2:$A$67</c:f>
               <c:strCache>
                 <c:ptCount val="66"/>
                 <c:pt idx="0">
@@ -1634,7 +1709,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>sismos_Brazil!$B$2:$B$67</c:f>
+              <c:f>'ORDEM DE DATA - GRÁFICOS'!$B$2:$B$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="66"/>
@@ -1849,11 +1924,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="1555391"/>
-        <c:axId val="94647626"/>
+        <c:axId val="65747193"/>
+        <c:axId val="61876619"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1555391"/>
+        <c:axId val="65747193"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1881,14 +1956,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94647626"/>
+        <c:crossAx val="61876619"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94647626"/>
+        <c:axId val="61876619"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1925,7 +2000,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1555391"/>
+        <c:crossAx val="65747193"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1990,7 +2065,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>sismos_Brazil!$A$2:$A$67</c:f>
+              <c:f>'ORDEM DE DATA - GRÁFICOS'!$A$2:$A$67</c:f>
               <c:strCache>
                 <c:ptCount val="66"/>
                 <c:pt idx="0">
@@ -2196,7 +2271,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>sismos_Brazil!$B$2:$B$67</c:f>
+              <c:f>'ORDEM DE DATA - GRÁFICOS'!$B$2:$B$67</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="66"/>
@@ -2411,11 +2486,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="34290125"/>
-        <c:axId val="13069997"/>
+        <c:axId val="78051583"/>
+        <c:axId val="10873843"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="34290125"/>
+        <c:axId val="78051583"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2452,14 +2527,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13069997"/>
+        <c:crossAx val="10873843"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="13069997"/>
+        <c:axId val="10873843"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2496,7 +2571,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34290125"/>
+        <c:crossAx val="78051583"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2534,9 +2609,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>561600</xdr:colOff>
+      <xdr:colOff>561240</xdr:colOff>
       <xdr:row>88</xdr:row>
-      <xdr:rowOff>109080</xdr:rowOff>
+      <xdr:rowOff>108720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2545,7 +2620,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="7219080" y="7821720"/>
-        <a:ext cx="11928960" cy="6710040"/>
+        <a:ext cx="11928600" cy="6709680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2564,9 +2639,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>504000</xdr:colOff>
+      <xdr:colOff>503640</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>82080</xdr:rowOff>
+      <xdr:rowOff>81720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2575,7 +2650,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="7330320" y="87120"/>
-        <a:ext cx="11760120" cy="6614640"/>
+        <a:ext cx="11759760" cy="6614280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2594,9 +2669,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>92520</xdr:colOff>
+      <xdr:colOff>92160</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>81720</xdr:rowOff>
+      <xdr:rowOff>81360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2605,7 +2680,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="12191760" y="2097360"/>
-        <a:ext cx="11363760" cy="6717240"/>
+        <a:ext cx="11363400" cy="6716880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2625,8 +2700,8 @@
   </sheetPr>
   <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3983,4 +4058,1382 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H67"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.68"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B32" s="1" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34" s="1" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B35" s="1" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B36" s="1" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="1" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="1" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="1" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" s="1" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="1" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="1" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="1" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B44" s="1" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="1" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B46" s="1" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" s="1" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B48" s="1" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" s="1" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B50" s="1" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="1" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52" s="1" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="1" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B54" s="1" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B55" s="1" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" s="1" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57" s="1" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B59" s="1" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B60" s="1" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B61" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B62" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B63" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B64" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B65" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F65" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B66" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E66" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B67" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" display="https://earthquake.usgs.gov/earthquakes/eventpage/*********/"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>